<commit_message>
Highlight issues in API Endpoints table
</commit_message>
<xml_diff>
--- a/project planning/API Endpoints.xlsx
+++ b/project planning/API Endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Resilio Sync\Daniel Schor\Studium\Module\Aktuell\WebApp\Projekt\Repo\webappproject23-24-devteam\project planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52BACE8C-129B-44F5-9B44-D8DA02A55016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1985AF29-6F28-46FC-9AF3-F8B769C9F940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9AEC6116-FBBD-4A6A-8287-4603E5F5CE05}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>No.</t>
   </si>
@@ -133,6 +133,25 @@
     <t>(keine zusätzlichen Header)
 (keine zusätzlichen Header)
 (keine zusätzlichen Header)</t>
+  </si>
+  <si>
+    <t>Zu
+ueberpruefen</t>
+  </si>
+  <si>
+    <t>Nicht
+richtig</t>
+  </si>
+  <si>
+    <t>Nicht
+fertig</t>
+  </si>
+  <si>
+    <t>Legende</t>
+  </si>
+  <si>
+    <t>Fertig /
+Richtig</t>
   </si>
 </sst>
 </file>
@@ -154,15 +173,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -238,22 +275,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -262,40 +320,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -306,12 +348,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -712,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9F2D08-239F-4D88-8E6A-1E4C636ABC07}">
-  <dimension ref="B3:G19"/>
+  <dimension ref="B3:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,291 +833,305 @@
     <col min="5" max="5" width="39.5703125" customWidth="1"/>
     <col min="6" max="6" width="29.140625" customWidth="1"/>
     <col min="7" max="7" width="45.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="9" t="s">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-      <c r="C4" s="10">
+    <row r="4" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="18">
         <v>1</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="11">
+    <row r="5" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+      <c r="C5" s="23">
         <v>2</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="30" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="11">
+    <row r="6" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="C6" s="23">
         <v>3</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="32" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="11">
+    <row r="7" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="8">
         <v>4</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="12">
+    <row r="8" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="26">
         <v>5</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="34" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="10">
+      <c r="I8" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+    </row>
+    <row r="9" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="18">
         <v>6</v>
       </c>
       <c r="D9" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="22" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="11">
+      <c r="I9" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+      <c r="C10" s="23">
         <v>7</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="30" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="11">
+    <row r="11" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="8">
         <v>8</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="11">
+    <row r="12" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="23">
         <v>9</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="32" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="11">
+    <row r="13" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="8">
         <v>10</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="23"/>
-      <c r="C14" s="12">
+    <row r="14" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="C14" s="26">
         <v>11</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="34" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="23"/>
-      <c r="C15" s="22">
+    <row r="15" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="C15" s="15">
         <v>12</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="23"/>
-      <c r="C16" s="22">
+    <row r="16" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="C16" s="15">
         <v>13</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
-      <c r="C17" s="12">
+      <c r="B17" s="6"/>
+      <c r="C17" s="9">
         <v>14</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I8:L8"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>